<commit_message>
fix: some minor things
</commit_message>
<xml_diff>
--- a/test/test_cases/tc0004CUPerCellCalc.xlsx
+++ b/test/test_cases/tc0004CUPerCellCalc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\cpp\newBUSTools\bustools\test\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E084F84-E6C7-42FC-893B-57B1879CED14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A55AB7-1CC3-47FC-9B90-D1E7B3BB859C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2985" yWindow="480" windowWidth="25170" windowHeight="14715" xr2:uid="{A85F2582-0153-482F-95D2-451F431EDD8F}"/>
   </bookViews>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E17ECC-2CEE-4E31-915B-746929019A18}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>